<commit_message>
Day Log: Refined the databases and items by converting Stock into a container for a StockItem model which holds item data inside a stock. Created functionality in the django admin site to make adding, deleting and modifying data easier and readable. Will commit more frequently as tasks complete instead of daily.
</commit_message>
<xml_diff>
--- a/media/Wiggle_Worm-Items.xlsx
+++ b/media/Wiggle_Worm-Items.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82345195-CBBB-490A-BEC0-06983DAC9A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90B9E62C-47BF-4A57-8E2C-F3AD26174E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Item Name</t>
+    <t>Item Id</t>
   </si>
   <si>
     <t>Item Weight</t>
@@ -449,7 +449,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15.75"/>

</xml_diff>